<commit_message>
excel file has been modified
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,23 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="family">Sheet1!$A$1:$E$5</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age </t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>mohamed</t>
+  </si>
+  <si>
+    <t>ahmed</t>
+  </si>
+  <si>
+    <t>eslam</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +54,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DE38D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,18 +84,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8DE38D"/>
+      <color rgb="FF66FF33"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +421,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E3" si="0">SUM(B2+C2+D2)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1021604302</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1579751216</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1150116220</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>500</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>160</v>
+      </c>
+      <c r="E4" s="3">
+        <f>SUM(B4+C4+D4)</f>
+        <v>1660</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>